<commit_message>
Refactors data retrieval and formatting
Refactors the SQL queries for improved data retrieval and reporting.

This includes adjustments to data aggregation, filtering, and formatting to ensure accuracy and consistency.
Also includes fixing issues related to account balance calculations and report generation.
Addresses date handling and reconciliation logic for improved accuracy in financial reporting.
</commit_message>
<xml_diff>
--- a/인천보고서_202502.xlsx
+++ b/인천보고서_202502.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\sidogeumgo\src\md\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14720573-F50E-4FD9-9BC5-45798B3CEEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0299D7-4E96-4CCE-B8A9-BDAC4817ECEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="110">
   <si>
     <t>품질관리 상세근거</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -585,6 +585,38 @@
   <si>
     <t>이호조 세입세출일계표 수정
 - 기산일 재전송 기능 수정 및 테스트</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>금고운용현황 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>지방재정 파일 재전송</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>예금운용현황 자료 검증</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>원주직인 추가</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2금고 자료 검증</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>수입증지 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>일괄잔액대사표 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 오류 원인 분석</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1359,6 +1391,42 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1410,46 +1478,10 @@
     <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1768,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B41" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B4" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1786,42 +1818,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="68" t="s">
+      <c r="B3" s="79"/>
+      <c r="C3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
@@ -1850,43 +1882,43 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="391.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="81" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="76" t="s">
+      <c r="E5" s="86"/>
+      <c r="F5" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="76" t="s">
+      <c r="G5" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="60"/>
+      <c r="H5" s="72"/>
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="70"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="61"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="73"/>
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="70"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="11" t="s">
         <v>50</v>
       </c>
@@ -1905,8 +1937,10 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="70"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" s="51" t="s">
         <v>25</v>
       </c>
@@ -1922,7 +1956,7 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="70"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="11" t="s">
         <v>52</v>
       </c>
@@ -1945,8 +1979,10 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="70"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="C10" s="51" t="s">
         <v>29</v>
       </c>
@@ -1962,7 +1998,7 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="70"/>
+      <c r="A11" s="82"/>
       <c r="B11" s="11" t="s">
         <v>52</v>
       </c>
@@ -1981,8 +2017,10 @@
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="70"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="11" t="s">
+        <v>102</v>
+      </c>
       <c r="C12" s="51" t="s">
         <v>31</v>
       </c>
@@ -1998,7 +2036,7 @@
       <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="70"/>
+      <c r="A13" s="82"/>
       <c r="B13" s="11" t="s">
         <v>52</v>
       </c>
@@ -2017,8 +2055,10 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="312.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="70"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="11" t="s">
+        <v>102</v>
+      </c>
       <c r="C14" s="51" t="s">
         <v>32</v>
       </c>
@@ -2034,7 +2074,7 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="70"/>
+      <c r="A15" s="82"/>
       <c r="B15" s="11" t="s">
         <v>54</v>
       </c>
@@ -2053,8 +2093,10 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="70"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="C16" s="51" t="s">
         <v>34</v>
       </c>
@@ -2070,8 +2112,10 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="70"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="C17" s="49" t="s">
         <v>35</v>
       </c>
@@ -2087,7 +2131,7 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="70"/>
+      <c r="A18" s="82"/>
       <c r="B18" s="11" t="s">
         <v>52</v>
       </c>
@@ -2106,8 +2150,10 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" ht="330.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="70"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="82"/>
+      <c r="B19" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="C19" s="49" t="s">
         <v>36</v>
       </c>
@@ -2123,7 +2169,7 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="70"/>
+      <c r="A20" s="82"/>
       <c r="B20" s="11" t="s">
         <v>56</v>
       </c>
@@ -2142,8 +2188,10 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="70"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="82"/>
+      <c r="B21" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="C21" s="49" t="s">
         <v>37</v>
       </c>
@@ -2162,7 +2210,7 @@
       <c r="H21" s="47"/>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="70"/>
+      <c r="A22" s="82"/>
       <c r="B22" s="11" t="s">
         <v>59</v>
       </c>
@@ -2184,8 +2232,10 @@
       <c r="H22" s="47"/>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="70"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="82"/>
+      <c r="B23" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="C23" s="49" t="s">
         <v>38</v>
       </c>
@@ -2223,7 +2273,9 @@
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" ht="167.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="48"/>
-      <c r="B25" s="11"/>
+      <c r="B25" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="C25" s="49" t="s">
         <v>39</v>
       </c>
@@ -2275,7 +2327,9 @@
     </row>
     <row r="28" spans="1:10" s="1" customFormat="1" ht="283.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="48"/>
-      <c r="B28" s="28"/>
+      <c r="B28" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="C28" s="49" t="s">
         <v>41</v>
       </c>
@@ -2309,7 +2363,9 @@
     </row>
     <row r="30" spans="1:10" s="1" customFormat="1" ht="207.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="48"/>
-      <c r="B30" s="28"/>
+      <c r="B30" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="C30" s="49" t="s">
         <v>42</v>
       </c>
@@ -2343,7 +2399,9 @@
     </row>
     <row r="32" spans="1:10" s="1" customFormat="1" ht="265.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="48"/>
-      <c r="B32" s="28"/>
+      <c r="B32" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="C32" s="49" t="s">
         <v>43</v>
       </c>
@@ -2377,7 +2435,9 @@
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="48"/>
-      <c r="B34" s="28"/>
+      <c r="B34" s="28" t="s">
+        <v>104</v>
+      </c>
       <c r="C34" s="49" t="s">
         <v>44</v>
       </c>
@@ -2411,7 +2471,9 @@
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="48"/>
-      <c r="B36" s="28"/>
+      <c r="B36" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="C36" s="49" t="s">
         <v>45</v>
       </c>
@@ -2445,7 +2507,9 @@
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="48"/>
-      <c r="B38" s="28"/>
+      <c r="B38" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="C38" s="49" t="s">
         <v>46</v>
       </c>
@@ -2461,7 +2525,9 @@
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="48"/>
-      <c r="B39" s="28"/>
+      <c r="B39" s="28" t="s">
+        <v>68</v>
+      </c>
       <c r="C39" s="49" t="s">
         <v>96</v>
       </c>
@@ -2477,7 +2543,9 @@
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="48"/>
-      <c r="B40" s="28"/>
+      <c r="B40" s="28" t="s">
+        <v>103</v>
+      </c>
       <c r="C40" s="49" t="s">
         <v>96</v>
       </c>
@@ -2529,7 +2597,9 @@
     </row>
     <row r="43" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="48"/>
-      <c r="B43" s="28"/>
+      <c r="B43" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="C43" s="49" t="s">
         <v>99</v>
       </c>
@@ -2554,19 +2624,19 @@
       <c r="H44" s="57"/>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="62" t="s">
+      <c r="A45" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="81" t="s">
+      <c r="B45" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="77" t="s">
+      <c r="C45" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="80" t="s">
+      <c r="D45" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="81" t="s">
+      <c r="E45" s="90" t="s">
         <v>79</v>
       </c>
       <c r="F45" s="24" t="s">
@@ -2578,21 +2648,21 @@
       <c r="H45" s="25"/>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="62"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
-      <c r="E46" s="82"/>
+      <c r="A46" s="74"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="64"/>
       <c r="F46" s="24"/>
       <c r="G46" s="24"/>
       <c r="H46" s="25"/>
     </row>
     <row r="47" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="62"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="82"/>
+      <c r="A47" s="74"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="64"/>
       <c r="F47" s="13" t="s">
         <v>15</v>
       </c>
@@ -2602,17 +2672,17 @@
       <c r="H47" s="15"/>
     </row>
     <row r="48" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="62"/>
-      <c r="B48" s="83"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="79"/>
-      <c r="E48" s="83"/>
+      <c r="A48" s="74"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="65"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="15"/>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="62"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="11"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
@@ -2626,7 +2696,7 @@
       <c r="H49" s="15"/>
     </row>
     <row r="50" spans="1:8" s="1" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="62"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="28"/>
       <c r="C50" s="50"/>
       <c r="D50" s="50"/>
@@ -2636,19 +2706,19 @@
       <c r="H50" s="33"/>
     </row>
     <row r="51" spans="1:8" s="41" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="84" t="s">
+      <c r="A51" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B51" s="87" t="s">
+      <c r="B51" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="77" t="s">
+      <c r="C51" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="77" t="s">
+      <c r="D51" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="E51" s="88" t="s">
+      <c r="E51" s="69" t="s">
         <v>27</v>
       </c>
       <c r="F51" s="39" t="s">
@@ -2660,21 +2730,21 @@
       <c r="H51" s="40"/>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="85"/>
-      <c r="B52" s="82"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="78"/>
-      <c r="E52" s="89"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="70"/>
       <c r="F52" s="24"/>
       <c r="G52" s="24"/>
       <c r="H52" s="25"/>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="85"/>
-      <c r="B53" s="82"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="78"/>
-      <c r="E53" s="89"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="70"/>
       <c r="F53" s="13" t="s">
         <v>15</v>
       </c>
@@ -2684,17 +2754,17 @@
       <c r="H53" s="15"/>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="85"/>
-      <c r="B54" s="83"/>
-      <c r="C54" s="79"/>
-      <c r="D54" s="79"/>
-      <c r="E54" s="90"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="68"/>
+      <c r="D54" s="68"/>
+      <c r="E54" s="71"/>
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="15"/>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="85"/>
+      <c r="A55" s="61"/>
       <c r="B55" s="11"/>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
@@ -2708,7 +2778,7 @@
       <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="85"/>
+      <c r="A56" s="61"/>
       <c r="B56" s="11"/>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
@@ -2718,7 +2788,7 @@
       <c r="H56" s="15"/>
     </row>
     <row r="57" spans="1:8" s="27" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="86"/>
+      <c r="A57" s="62"/>
       <c r="B57" s="17"/>
       <c r="C57" s="42"/>
       <c r="D57" s="42"/>
@@ -2893,11 +2963,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="E51:E54"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="A45:A50"/>
     <mergeCell ref="A1:H1"/>
@@ -2914,6 +2979,11 @@
     <mergeCell ref="D45:D48"/>
     <mergeCell ref="E45:E48"/>
     <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="E51:E54"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.3" right="0" top="0.3" bottom="0.11811023622047245" header="0.22" footer="0.19685039370078741"/>

</xml_diff>